<commit_message>
added method to build final excel file and delete csv files
</commit_message>
<xml_diff>
--- a/reports_project/Old_Month_Report/DEF_Old_report.xlsx
+++ b/reports_project/Old_Month_Report/DEF_Old_report.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11116"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12626380-6B51-6C45-BCD1-E1E69AC363BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87364F67-0201-7645-9A28-AC273A73084A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12120" yWindow="8220" windowWidth="23440" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12120" yWindow="8220" windowWidth="23440" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CLP" sheetId="9" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="60">
   <si>
     <t>Name</t>
   </si>
@@ -138,9 +138,6 @@
   </si>
   <si>
     <t>Employee Name</t>
-  </si>
-  <si>
-    <t>Column1</t>
   </si>
   <si>
     <t>Notes</t>
@@ -2261,9 +2258,6 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C402898B-1F29-46AE-93E4-650D764269AA}" name="Table1" displayName="Table1" ref="A1:T16" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51" tableBorderDxfId="50">
   <autoFilter ref="A1:T16" xr:uid="{C402898B-1F29-46AE-93E4-650D764269AA}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:T1">
-    <sortCondition ref="M1"/>
-  </sortState>
   <tableColumns count="20">
     <tableColumn id="20" xr3:uid="{DC3981F6-48D7-44CC-AF77-104F5D0C8002}" name="Notes" dataDxfId="49"/>
     <tableColumn id="1" xr3:uid="{C7725C49-BB83-4C9A-A839-3E1F0BD0EF85}" name="ORG CODE" dataDxfId="48"/>
@@ -2307,7 +2301,7 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="14">
-    <tableColumn id="14" xr3:uid="{452B8F95-B4FF-47FA-A2CD-558844FD14E3}" name="Column1" dataDxfId="26"/>
+    <tableColumn id="14" xr3:uid="{452B8F95-B4FF-47FA-A2CD-558844FD14E3}" name="Notes" dataDxfId="26"/>
     <tableColumn id="1" xr3:uid="{F9AF80B6-6878-4BA0-BAD5-DCEE169549F7}" name="ORG_CODE" dataDxfId="25"/>
     <tableColumn id="2" xr3:uid="{3977BD6E-118A-4EE5-AF0A-553AA0A2C879}" name="Employee Name" dataDxfId="24"/>
     <tableColumn id="3" xr3:uid="{9C44D2D0-F2B5-4B21-958A-2DB3CB909B06}" name="APPNT EFF DATE" dataDxfId="23"/>
@@ -2650,7 +2644,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA8147FA-A521-46E2-B8DB-CF7C8B7F7D75}">
   <dimension ref="A1:T16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -2677,7 +2671,7 @@
   <sheetData>
     <row r="1" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>8</v>
@@ -2739,13 +2733,13 @@
     </row>
     <row r="2" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
         <v>39</v>
-      </c>
-      <c r="B2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" t="s">
-        <v>40</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
@@ -2769,13 +2763,13 @@
     </row>
     <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" t="s">
         <v>41</v>
-      </c>
-      <c r="C3" t="s">
-        <v>42</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
@@ -2800,10 +2794,10 @@
     <row r="4" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
@@ -2827,13 +2821,13 @@
     </row>
     <row r="5" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
@@ -2857,13 +2851,13 @@
     </row>
     <row r="6" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
@@ -2887,13 +2881,13 @@
     </row>
     <row r="7" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
@@ -2917,13 +2911,13 @@
     </row>
     <row r="8" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
@@ -2947,13 +2941,13 @@
     </row>
     <row r="9" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
@@ -2978,10 +2972,10 @@
     <row r="10" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8"/>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
@@ -3005,13 +2999,13 @@
     </row>
     <row r="11" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
@@ -3035,13 +3029,13 @@
     </row>
     <row r="12" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
@@ -3065,13 +3059,13 @@
     </row>
     <row r="13" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
@@ -3095,13 +3089,13 @@
     </row>
     <row r="14" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
@@ -3125,13 +3119,13 @@
     </row>
     <row r="15" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
@@ -3155,13 +3149,13 @@
     </row>
     <row r="16" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
@@ -3196,8 +3190,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF21CF73-D586-4E45-8A55-9C7E858C8B75}">
   <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3264,10 +3258,10 @@
     <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="14"/>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D2" s="15">
         <v>45296</v>
@@ -3286,13 +3280,13 @@
     </row>
     <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" t="s">
         <v>41</v>
-      </c>
-      <c r="C3" t="s">
-        <v>42</v>
       </c>
       <c r="D3" s="15">
         <v>45318</v>
@@ -3311,10 +3305,10 @@
     <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="19"/>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D4" s="15">
         <v>45489</v>
@@ -3332,13 +3326,13 @@
     </row>
     <row r="5" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D5" s="15">
         <v>45570</v>
@@ -3420,7 +3414,7 @@
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -3432,13 +3426,13 @@
       </c>
       <c r="H2" s="13"/>
       <c r="I2" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J2" s="12"/>
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
@@ -3450,7 +3444,7 @@
       </c>
       <c r="H3" s="13"/>
       <c r="I3" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J3" s="12"/>
     </row>
@@ -3469,53 +3463,16 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocIdPersistId xmlns="bf465682-a195-48e8-a373-685144231e9c">true</_dlc_DocIdPersistId>
+    <_dlc_DocId xmlns="bf465682-a195-48e8-a373-685144231e9c">WCVJDXXHMT7D-945044613-85</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="bf465682-a195-48e8-a373-685144231e9c">
+      <Url>https://cisgov.sharepoint.com/sites/ECNhct/Offices/hct/HRIT/HCTReportingCenter/_layouts/15/DocIdRedir.aspx?ID=WCVJDXXHMT7D-945044613-85</Url>
+      <Description>WCVJDXXHMT7D-945044613-85</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3693,16 +3650,53 @@
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocIdPersistId xmlns="bf465682-a195-48e8-a373-685144231e9c">true</_dlc_DocIdPersistId>
-    <_dlc_DocId xmlns="bf465682-a195-48e8-a373-685144231e9c">WCVJDXXHMT7D-945044613-85</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="bf465682-a195-48e8-a373-685144231e9c">
-      <Url>https://cisgov.sharepoint.com/sites/ECNhct/Offices/hct/HRIT/HCTReportingCenter/_layouts/15/DocIdRedir.aspx?ID=WCVJDXXHMT7D-945044613-85</Url>
-      <Description>WCVJDXXHMT7D-945044613-85</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3714,9 +3708,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D16E658-4C8F-4C0E-B7D2-CFF9B31601AF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9DE39C24-384E-4C44-9878-44FE0A7BA72C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="c5ed04f4-622d-4734-9b15-89f52925a551"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="bf465682-a195-48e8-a373-685144231e9c"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3741,18 +3744,9 @@
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9DE39C24-384E-4C44-9878-44FE0A7BA72C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D16E658-4C8F-4C0E-B7D2-CFF9B31601AF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="c5ed04f4-622d-4734-9b15-89f52925a551"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="bf465682-a195-48e8-a373-685144231e9c"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>